<commit_message>
System workbench - c 및 header file 추가 및 경로 설정 방법 추가
</commit_message>
<xml_diff>
--- a/STM32Cube Data/STM32 System Workbench Manual.xlsx
+++ b/STM32Cube Data/STM32 System Workbench Manual.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="program DL" sheetId="1" r:id="rId1"/>
     <sheet name="Install" sheetId="2" r:id="rId2"/>
-    <sheet name="사용법" sheetId="3" r:id="rId3"/>
+    <sheet name="Project path 설정" sheetId="3" r:id="rId3"/>
+    <sheet name="c 및 header file 추가" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>http://www.openstm32.org/System%2BWorkbench%2Bfor%2BSTM32</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -154,7 +155,130 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4. Compile - Project &gt; Build All를 선택한다.</t>
+    <t>4. Compile - Project &gt; Clean 과 Build All를 차례로 실행시킨다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. 위와 같이 실행 후에도 Project open이 안되는 경우 아래와 같이 파일을 삭제 후 위 순서대로 실행함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Project folder에서 마우슨 오른쪽 pop-up후 Delete를 선택 후 위와 같이 다시 실행함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1) 아래와 같이 Src folder에 추가하고자 하는 .c file과 .h file을 복사한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2) 탐색기에서 Copy한 아래 folder 및 file들을 마우스로 끌어서 WorkBench의 Application folder에 추가한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3) 아래와 같은 Pop-up이 뜨면, Link to files and folders를 선택하고 OK한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탐색기에서 file은 먼저 copy를 했으므로, Link만 시키면 된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Includes 파일 path 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1) Project에서 마우스 오른쪽 pop-up을 실행하고, Properties를 선택함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2) C/C++ Build &gt; Settings을 선택함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3) MCU GCC Compiler &gt; Includes 선택함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4) WorkBench의 기준 경로는 아래와 같이 Plasma_Gen_V1.0_20171227 ( Cube로 generation된 SW4STM32 하위 folder)를 기준으로 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>즉, 위와 같이 Inc의 경로는 Plasma_Gen_V1.0_20171227 기준으로 상위 3번째 folder이므로 ../../../Inc가 된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Src에 추가된 file들에 대한 include 경로를 추가하기 위해서는 ../../../Src/에 추가된 folder 경로를 추가하면 된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5) Plasma_Gen_V1.0_20171227\Src\Application\CliTask folder의 file의 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Includes paths(-I)의 + Icon를 선택 후 Add directory path에 아래와 같이 경로를 추가한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Gen_V1.0_20171227\Src\Application\CliTask folder의 file이 추가된 상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6) 5와 같은 방법으로 아래 경로들을 추가한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Gen_V1.0_20171227\Src\Application\common</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Gen_V1.0_20171227\Src\Application\InEventTask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Gen_V1.0_20171227\Src\Application\mctask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Gen_V1.0_20171227\Src\Application\OutEventTask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Gen_V1.0_20171227\Src\Application\taskcfg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Gen_V1.0_20171227\Src\Application</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Gen_V1.0_20171227\Src\Application\InEventTask\ADC</t>
+  </si>
+  <si>
+    <t>Plasma_Gen_V1.0_20171227\Src\Application\OutEventTask\Buzzer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Gen_V1.0_20171227\Src\Application\OutEventTask\ChargeState</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Plasma_Gen_V1.0_20171227\Src\Application\OutEventTask\Plasma</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>folder는 모두 경로를 추가해야 하므로, 하위 folder가 있는 Path는 아래와 같이 구별하여 추가해야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7) Include file이 추가된 WorkBench 상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8) Project&gt;Clean 및 Build All를 차례대로 선택하여 Compile error가 없는지 확인한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. C file 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -162,7 +286,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +318,13 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -216,10 +347,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1641,6 +1773,1383 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="그림 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="885825" y="17897475"/>
+          <a:ext cx="5572125" cy="3838575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>602712</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="9" name="그룹 8"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="685801" y="466725"/>
+          <a:ext cx="8679911" cy="3590925"/>
+          <a:chOff x="691663" y="472587"/>
+          <a:chExt cx="8718011" cy="3640748"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="3" name="그림 2"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="691663" y="482112"/>
+            <a:ext cx="4169861" cy="3631223"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="8" name="그룹 7"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="4979377" y="472587"/>
+            <a:ext cx="4430297" cy="3621698"/>
+            <a:chOff x="4979377" y="472587"/>
+            <a:chExt cx="4430297" cy="3621698"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="5" name="그림 4"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:srcRect/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="4979377" y="472587"/>
+              <a:ext cx="4430297" cy="3621698"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="모서리가 둥근 직사각형 5"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7691804" y="1362076"/>
+              <a:ext cx="1587012" cy="235194"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="오른쪽 화살표 6"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4593981" y="1370135"/>
+            <a:ext cx="608134" cy="520211"/>
+          </a:xfrm>
+          <a:prstGeom prst="rightArrow">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="17" name="그룹 16"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="638175" y="4695826"/>
+          <a:ext cx="8620125" cy="7896224"/>
+          <a:chOff x="638175" y="4695826"/>
+          <a:chExt cx="8620125" cy="7896224"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="11" name="그림 10"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="676275" y="4695826"/>
+            <a:ext cx="8582025" cy="3467568"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="13" name="그림 12"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="638175" y="8248650"/>
+            <a:ext cx="5572125" cy="4343400"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="14" name="모서리가 둥근 직사각형 13"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4048125" y="5753100"/>
+            <a:ext cx="5048249" cy="1771650"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="16" name="직선 화살표 연결선 15"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="1962150" y="7572375"/>
+            <a:ext cx="2505075" cy="2000250"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="38100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>294779</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>9219</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="그림 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="971550" y="13277850"/>
+          <a:ext cx="3971429" cy="2447619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>313</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>321</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="모서리가 둥근 직사각형 21"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2514600" y="65627251"/>
+          <a:ext cx="5048249" cy="1771650"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="25" name="그룹 24"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="962025" y="15982950"/>
+          <a:ext cx="5295900" cy="5676900"/>
+          <a:chOff x="962025" y="15982950"/>
+          <a:chExt cx="5295900" cy="5676900"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="21" name="그림 20"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="962025" y="15982950"/>
+            <a:ext cx="5295900" cy="5676900"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="23" name="모서리가 둥근 직사각형 22"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1095376" y="17268826"/>
+            <a:ext cx="1809750" cy="1057274"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="24" name="모서리가 둥근 직사각형 23"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1085851" y="18497551"/>
+            <a:ext cx="1809750" cy="200024"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="그림 26"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="22488525"/>
+          <a:ext cx="5067300" cy="2371725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>103431</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="그림 27"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="971550" y="25241250"/>
+          <a:ext cx="8372475" cy="5037381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>90192</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="그림 28"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="942975" y="30641926"/>
+          <a:ext cx="8429625" cy="5071766"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>193</xdr:row>
+      <xdr:rowOff>88720</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="35" name="그룹 34"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="990600" y="36547425"/>
+          <a:ext cx="8353425" cy="3984445"/>
+          <a:chOff x="990600" y="36547425"/>
+          <a:chExt cx="8353425" cy="3984445"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="31" name="그림 30"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="990600" y="36547425"/>
+            <a:ext cx="8353425" cy="3984445"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="32" name="TextBox 31"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1533525" y="39528750"/>
+            <a:ext cx="409575" cy="491417"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1800" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>①</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1800" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="33" name="TextBox 32"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1438275" y="39290625"/>
+            <a:ext cx="314325" cy="491417"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1800" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>②</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1800" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="34" name="TextBox 33"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1362075" y="37947600"/>
+            <a:ext cx="314325" cy="491417"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1800" b="1">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>③</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1800" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>638176</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>99061</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="39" name="그룹 38"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="981076" y="41148001"/>
+          <a:ext cx="8420100" cy="5052060"/>
+          <a:chOff x="914400" y="41281350"/>
+          <a:chExt cx="9191625" cy="5514975"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="37" name="그림 36"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="914400" y="41281350"/>
+            <a:ext cx="9191625" cy="5514975"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="38" name="모서리가 둥근 직사각형 37"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8420101" y="41909999"/>
+            <a:ext cx="342900" cy="304801"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>222</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>246</xdr:row>
+      <xdr:rowOff>59601</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="그림 39"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="971550" y="46577251"/>
+          <a:ext cx="8362950" cy="5031650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>259</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>283</xdr:row>
+      <xdr:rowOff>51934</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="그림 41"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1000125" y="54130576"/>
+          <a:ext cx="8334375" cy="5014458"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66676</xdr:colOff>
+      <xdr:row>285</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>638176</xdr:colOff>
+      <xdr:row>308</xdr:row>
+      <xdr:rowOff>21335</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="46" name="그룹 45"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="676276" y="59769375"/>
+          <a:ext cx="8724900" cy="4793360"/>
+          <a:chOff x="676276" y="59769375"/>
+          <a:chExt cx="8724900" cy="4793360"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="44" name="그림 43"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="676276" y="59769375"/>
+            <a:ext cx="8724900" cy="4793360"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="45" name="모서리가 둥근 직사각형 44"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="914400" y="62636401"/>
+            <a:ext cx="3781425" cy="1552574"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2126,10 +3635,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C64"/>
+  <dimension ref="B2:C85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="R77" sqref="R77"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="L107" sqref="L107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2163,9 +3672,193 @@
         <v>34</v>
       </c>
     </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C85" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:K310"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U32" sqref="U32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="3" width="4" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C22" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C62" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D63" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B106" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C107" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C120" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C146" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="172" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C172" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="173" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D173" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="174" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D174" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="195" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C195" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="196" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D196" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="198" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="D198" s="2"/>
+    </row>
+    <row r="199" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="K199" s="3"/>
+    </row>
+    <row r="222" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D222" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="248" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C248" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="249" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D249" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="250" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D250" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="251" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D251" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="252" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D252" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="253" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D253" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="254" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D254" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="255" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D255" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="256" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D256" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="257" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D257" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="258" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D258" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="259" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D259" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="285" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C285" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="310" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C310" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
System workbench manual - debug sheet 추가
</commit_message>
<xml_diff>
--- a/STM32Cube Data/STM32 System Workbench Manual.xlsx
+++ b/STM32Cube Data/STM32 System Workbench Manual.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="program DL" sheetId="1" r:id="rId1"/>
     <sheet name="Install" sheetId="2" r:id="rId2"/>
     <sheet name="Project path 설정" sheetId="3" r:id="rId3"/>
     <sheet name="c 및 header file 추가" sheetId="4" r:id="rId4"/>
+    <sheet name="Debug" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>http://www.openstm32.org/System%2BWorkbench%2Bfor%2BSTM32</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -279,6 +280,14 @@
   </si>
   <si>
     <t>1. C file 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Debug 설정 방법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 확인하고자 하는 위치에 break</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3153,6 +3162,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>141238</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>132312</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="419100"/>
+          <a:ext cx="13095238" cy="8304762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -3693,8 +3745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U32" sqref="U32"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3861,4 +3913,34 @@
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X16" sqref="X16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="4" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
System workbench manual - debug 설명 추가
</commit_message>
<xml_diff>
--- a/STM32Cube Data/STM32 System Workbench Manual.xlsx
+++ b/STM32Cube Data/STM32 System Workbench Manual.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>http://www.openstm32.org/System%2BWorkbench%2Bfor%2BSTM32</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -287,7 +287,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1. 확인하고자 하는 위치에 break</t>
+    <t>ST Link와 board를 SWD 연결한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reset pin이 연결되어 있지 않다면, Board가 항상 On을 유지하도록 USB 또는 전원Key를 누르고 있는다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Board의 S/W와 Source는 동일해야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 확인하고자 하는 위치에 breakpoint를 추가하고, debug 버튼을 선택한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. debug를 실행하면 아래와 같이 화면이 display되며, 처음 breakpoint에서 정지된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>system init 부분에 debug start point로 breakpooint가 하나는 있어야 한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3164,42 +3184,381 @@
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>107674</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>41412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>563218</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>173933</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="모서리가 둥근 직사각형 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10270435" y="7495760"/>
+          <a:ext cx="455544" cy="339586"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>141238</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>132312</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>102296</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="10" name="그룹 9"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="609600" y="419100"/>
-          <a:ext cx="13095238" cy="8304762"/>
+          <a:off x="689113" y="1082952"/>
+          <a:ext cx="8698810" cy="5438366"/>
+          <a:chOff x="689113" y="1082952"/>
+          <a:chExt cx="8698810" cy="5438366"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="6" name="그룹 5"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="689113" y="1082952"/>
+            <a:ext cx="8698810" cy="5438366"/>
+            <a:chOff x="689113" y="461756"/>
+            <a:chExt cx="8698810" cy="5438366"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="3" name="그림 2"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="689113" y="461756"/>
+              <a:ext cx="8698810" cy="5438366"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="모서리가 둥근 직사각형 4"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2637182" y="2363857"/>
+              <a:ext cx="319709" cy="1280491"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3109291" y="1378225"/>
+            <a:ext cx="336274" cy="245166"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="12700">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>8282</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>49696</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>512</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="13" name="그룹 12"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="621195" y="7089913"/>
+          <a:ext cx="8738152" cy="5541577"/>
+          <a:chOff x="612913" y="6833152"/>
+          <a:chExt cx="8738152" cy="5541577"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="11" name="그룹 10"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="612913" y="6833152"/>
+            <a:ext cx="8738152" cy="5541577"/>
+            <a:chOff x="612913" y="6833152"/>
+            <a:chExt cx="8738152" cy="5541577"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="7" name="그림 6"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="612913" y="6833152"/>
+              <a:ext cx="8738152" cy="5541577"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="모서리가 둥근 직사각형 7"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8849139" y="7084943"/>
+              <a:ext cx="455544" cy="339586"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="12" name="모서리가 둥근 직사각형 11"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="674204" y="9503464"/>
+            <a:ext cx="1553817" cy="236884"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="12700">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3917,10 +4276,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C2"/>
+  <dimension ref="B1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S45" sqref="S45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3938,9 +4297,35 @@
         <v>67</v>
       </c>
     </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
System workbench manual - debug 설명 추가 완료
</commit_message>
<xml_diff>
--- a/STM32Cube Data/STM32 System Workbench Manual.xlsx
+++ b/STM32Cube Data/STM32 System Workbench Manual.xlsx
@@ -13,12 +13,15 @@
     <sheet name="c 및 header file 추가" sheetId="4" r:id="rId4"/>
     <sheet name="Debug" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Debug!$A$1:$Q$68</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>http://www.openstm32.org/System%2BWorkbench%2Bfor%2BSTM32</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -287,27 +290,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ST Link와 board를 SWD 연결한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reset pin이 연결되어 있지 않다면, Board가 항상 On을 유지하도록 USB 또는 전원Key를 누르고 있는다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Board의 S/W와 Source는 동일해야 한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 확인하고자 하는 위치에 breakpoint를 추가하고, debug 버튼을 선택한다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2. debug를 실행하면 아래와 같이 화면이 display되며, 처음 breakpoint에서 정지된다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>system init 부분에 debug start point로 breakpooint가 하나는 있어야 한다.</t>
+    <t>1. ST Link와 board를 SWD 연결한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. Board에 Source download하여 Version을 통일한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. reset pin이 연결되어 있지 않다면, Board가 항상 On을 유지하도록 USB 또는 전원Key를 누르고 있는다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. system init 부분에 debug start point로 breakpooint를 추가하고, Debug를 실행한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. debug를 실행하면 아래와 같이 화면이 display되며, 처음 breakpoint에서 정지된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6. 확인하고자 하는 위치에 breakpoint를 추가하고, Monitor하고자하는 변수를 마우스로 끌어다 Express에 추가한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7. Resume 버튼을 선택하면, Expression의 value가 update된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Step Into / Step Over / Step Return 버튼을 적절히 선택하여 Step별로 실행하며 debugging 한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3187,15 +3198,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>107674</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>41412</xdr:rowOff>
+      <xdr:colOff>463826</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>49695</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>563218</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>173933</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>231913</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>182215</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3204,7 +3215,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10270435" y="7495760"/>
+          <a:off x="10494065" y="17650238"/>
           <a:ext cx="455544" cy="339586"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -3247,46 +3258,46 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>22910</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:rowOff>41413</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>102296</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>42562</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>80132</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="10" name="그룹 9"/>
+        <xdr:cNvPr id="18" name="그룹 17"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="689113" y="1082952"/>
-          <a:ext cx="8698810" cy="5438366"/>
-          <a:chOff x="689113" y="1082952"/>
-          <a:chExt cx="8698810" cy="5438366"/>
+          <a:off x="809758" y="1076739"/>
+          <a:ext cx="8575587" cy="6664806"/>
+          <a:chOff x="809758" y="1076739"/>
+          <a:chExt cx="8575587" cy="6664806"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="6" name="그룹 5"/>
+          <xdr:cNvPr id="16" name="그룹 15"/>
           <xdr:cNvGrpSpPr/>
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="689113" y="1082952"/>
-            <a:ext cx="8698810" cy="5438366"/>
-            <a:chOff x="689113" y="461756"/>
-            <a:chExt cx="8698810" cy="5438366"/>
+            <a:off x="809758" y="1076739"/>
+            <a:ext cx="8575587" cy="6664806"/>
+            <a:chOff x="809757" y="1068457"/>
+            <a:chExt cx="8575587" cy="6664806"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="3" name="그림 2"/>
+            <xdr:cNvPr id="14" name="그림 13"/>
             <xdr:cNvPicPr>
               <a:picLocks noChangeAspect="1"/>
             </xdr:cNvPicPr>
@@ -3299,8 +3310,8 @@
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="689113" y="461756"/>
-              <a:ext cx="8698810" cy="5438366"/>
+              <a:off x="809757" y="1068457"/>
+              <a:ext cx="8575587" cy="6664806"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3309,13 +3320,13 @@
         </xdr:pic>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="5" name="모서리가 둥근 직사각형 4"/>
+            <xdr:cNvPr id="15" name="모서리가 둥근 직사각형 14"/>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2637182" y="2363857"/>
-              <a:ext cx="319709" cy="1280491"/>
+              <a:off x="2252870" y="3188804"/>
+              <a:ext cx="1474304" cy="265044"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
               <a:avLst/>
@@ -3356,13 +3367,13 @@
       </xdr:grpSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="9" name="모서리가 둥근 직사각형 8"/>
+          <xdr:cNvPr id="17" name="모서리가 둥근 직사각형 16"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="3109291" y="1378225"/>
-            <a:ext cx="336274" cy="245166"/>
+            <a:off x="3791497" y="1432891"/>
+            <a:ext cx="341525" cy="240196"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
             <a:avLst/>
@@ -3405,60 +3416,302 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>8282</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>49696</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>24848</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>57979</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>571499</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>512</xdr:rowOff>
+      <xdr:colOff>654326</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>36364</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="13" name="그룹 12"/>
+        <xdr:cNvPr id="21" name="그룹 20"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="621195" y="7089913"/>
-          <a:ext cx="8738152" cy="5541577"/>
-          <a:chOff x="612913" y="6833152"/>
-          <a:chExt cx="8738152" cy="5541577"/>
+          <a:off x="811696" y="8133522"/>
+          <a:ext cx="8497956" cy="6604472"/>
+          <a:chOff x="811696" y="8133522"/>
+          <a:chExt cx="8497956" cy="6604472"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="19" name="그림 18"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="811696" y="8133522"/>
+            <a:ext cx="8497956" cy="6604472"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="20" name="모서리가 둥근 직사각형 19"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="889550" y="11574116"/>
+            <a:ext cx="1719471" cy="236884"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="12700">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>33132</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>66260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>665955</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>152634</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="25" name="그룹 24"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="819980" y="15182021"/>
+          <a:ext cx="8501301" cy="6298330"/>
+          <a:chOff x="819980" y="15182021"/>
+          <a:chExt cx="8501301" cy="6298330"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="22" name="그림 21"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="819980" y="15182021"/>
+            <a:ext cx="8501301" cy="6298330"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="23" name="모서리가 둥근 직사각형 22"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="872986" y="18887660"/>
+            <a:ext cx="1413013" cy="253449"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="12700">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="24" name="모서리가 둥근 직사각형 23"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5088835" y="15748551"/>
+            <a:ext cx="3607904" cy="1297058"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="12700">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>33131</xdr:colOff>
+      <xdr:row>106</xdr:row>
+      <xdr:rowOff>74542</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>612913</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>121619</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="33" name="그룹 32"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="819979" y="22023455"/>
+          <a:ext cx="8448260" cy="6259034"/>
+          <a:chOff x="819979" y="22023455"/>
+          <a:chExt cx="8448260" cy="6259034"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="11" name="그룹 10"/>
+          <xdr:cNvPr id="31" name="그룹 30"/>
           <xdr:cNvGrpSpPr/>
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="612913" y="6833152"/>
-            <a:ext cx="8738152" cy="5541577"/>
-            <a:chOff x="612913" y="6833152"/>
-            <a:chExt cx="8738152" cy="5541577"/>
+            <a:off x="819979" y="22023455"/>
+            <a:ext cx="8448260" cy="6259034"/>
+            <a:chOff x="819979" y="21816390"/>
+            <a:chExt cx="8448260" cy="6259034"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="7" name="그림 6"/>
+            <xdr:cNvPr id="26" name="그림 25"/>
             <xdr:cNvPicPr>
               <a:picLocks noChangeAspect="1"/>
             </xdr:cNvPicPr>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="612913" y="6833152"/>
-              <a:ext cx="8738152" cy="5541577"/>
+              <a:off x="819979" y="21816390"/>
+              <a:ext cx="8448260" cy="6259034"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -3467,13 +3720,59 @@
         </xdr:pic>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="8" name="모서리가 둥근 직사각형 7"/>
+            <xdr:cNvPr id="27" name="모서리가 둥근 직사각형 26"/>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8849139" y="7084943"/>
-              <a:ext cx="455544" cy="339586"/>
+              <a:off x="7639878" y="22772202"/>
+              <a:ext cx="692425" cy="766971"/>
+            </a:xfrm>
+            <a:prstGeom prst="roundRect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="30" name="모서리가 둥근 직사각형 29"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2143540" y="22146038"/>
+              <a:ext cx="291548" cy="291550"/>
             </a:xfrm>
             <a:prstGeom prst="roundRect">
               <a:avLst/>
@@ -3514,13 +3813,13 @@
       </xdr:grpSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="12" name="모서리가 둥근 직사각형 11"/>
+          <xdr:cNvPr id="32" name="모서리가 둥근 직사각형 31"/>
           <xdr:cNvSpPr/>
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="674204" y="9503464"/>
-            <a:ext cx="1553817" cy="236884"/>
+            <a:off x="2799523" y="22354759"/>
+            <a:ext cx="692425" cy="289893"/>
           </a:xfrm>
           <a:prstGeom prst="roundRect">
             <a:avLst/>
@@ -4276,50 +4575,62 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C34"/>
+  <dimension ref="B1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S45" sqref="S45"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="4" customWidth="1"/>
+    <col min="1" max="1" width="2.25" customWidth="1"/>
+    <col min="2" max="3" width="4" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C39" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C73" s="2" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="105" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C105" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="106" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D106" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>